<commit_message>
tc 3 9 11 12 for bento perf
</commit_message>
<xml_diff>
--- a/InputFiles/TC03_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-TumorGrade.xlsx
+++ b/InputFiles/TC03_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-TumorGrade.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4277D5E5-4508-4196-85D6-F4217E29C3EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5920BD89-AE7D-4ED3-8505-D47DE7667A9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="610" windowWidth="19140" windowHeight="10190" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and d.tumor_grade In ["Not Reported"]
+WHERE ss.disease_subtype IN ["Mucinous (colloid) Carcinoma"] and sf.grouped_recurrence_score IN ["51-100"]and d.tumor_size_group In ["&gt;4"] and  d.tumor_grade In ["Intermediate Grade"]
 WITH ss
 MATCH (ss)-[:study_subject_of_study]-&gt;(s)
 MATCH (s)-[:study_of_program]-&gt;(p)
@@ -82,25 +82,26 @@
 COUNT(DISTINCT f) AS Files</t>
   </si>
   <si>
-    <t>MATCH (f:file)
-MATCH (f)-[:file_of_sample]-&gt;(samp)
-MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+    <t>MATCH (ss:study_subject)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
+WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (s)-[:study_of_program]-&gt;(p)
-MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
-MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and d.tumor_grade In ["Not Reported"]
-RETURN  f.file_name AS `File Name`,
-    head(labels(samp)) AS `Association`,
-    f.file_description AS `Description`,
-    f.file_format AS `File Format`,
-    f.file_size AS `Size`,
-    p.program_acronym AS `Program Code`,
-    s.study_acronym AS `Arm`,
-    ss.study_subject_id AS `Case ID`,
-    samp.sample_id AS `Sample ID`,
-    ss.disease_subtype as `Diagnosis`</t>
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
+MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
+WHERE ss.disease_subtype IN ["Mucinous (colloid) Carcinoma"] and sf.grouped_recurrence_score IN ["51-100"]and d.tumor_size_group In ["&gt;4"] and  d.tumor_grade In ["Intermediate Grade"]
+return ss.study_subject_id as `Case ID`,
+       p.program_acronym as `Program Code`,
+        p.program_id as Program_ID,
+       s.study_acronym as `Arm`,
+       ss.disease_subtype as `Diagnosis`,
+       sf.grouped_recurrence_score AS `Recurrence Score`,
+       d.tumor_size_group AS `tumor_size`,
+       d.er_status AS `ER Status`,
+       d.pr_status AS `PR Status`,
+       demo.age_at_index AS `Age (years)`,
+demo.survival_time AS `Survival (days)`</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
@@ -112,7 +113,7 @@
 MATCH (samp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and d.tumor_grade In ["Not Reported"]
+WHERE ss.disease_subtype IN ["Mucinous (colloid) Carcinoma"] and sf.grouped_recurrence_score IN ["51-100"]and d.tumor_size_group In ["&gt;4"] and  d.tumor_grade In ["Intermediate Grade"]
 WITH
     distinct lp,
     toInteger(split(ss.study_subject_id,'-')[2]) AS subject_id_num,
@@ -131,26 +132,25 @@
             lp.test_name as Platform</t>
   </si>
   <si>
-    <t>MATCH (ss:study_subject)
-MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
-WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
+    <t>MATCH (f:file)
+MATCH (f)-[:file_of_sample]-&gt;(samp)
+MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
- WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and d.tumor_grade In ["Not Reported"]
-return ss.study_subject_id as `Case ID`,
-       p.program_acronym as `Program Code`,
-        p.program_id as Program_ID,
-       s.study_acronym as `Arm`,
-       ss.disease_subtype as `Diagnosis`,
-       sf.grouped_recurrence_score AS `Recurrence Score`,
-       d.tumor_size_group AS `tumor_size`,
-       d.er_status AS `ER Status`,
-       d.pr_status AS `PR Status`,
-       demo.age_at_index AS `Age (years)`,
-demo.survival_time AS `Survival (days)`</t>
+MATCH (s)-[:study_of_program]-&gt;(p)
+MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
+MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
+WHERE ss.disease_subtype IN ["Mucinous (colloid) Carcinoma"] and sf.grouped_recurrence_score IN ["51-100"]and d.tumor_size_group In ["&gt;4"] and  d.tumor_grade In ["Intermediate Grade"]
+RETURN  f.file_name AS `File Name`,
+    head(labels(samp)) AS `Association`,
+    f.file_description AS `Description`,
+    f.file_format AS `File Format`,
+    f.file_size AS `Size`,
+    p.program_acronym AS `Program Code`,
+    s.study_acronym AS `Arm`,
+    ss.study_subject_id AS `Case ID`,
+    samp.sample_id AS `Sample ID`,
+    ss.disease_subtype as `Diagnosis`</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -591,7 +591,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>

</xml_diff>